<commit_message>
算法 V 0.3版本发布  修改了 ChargingDemo的版权信息 AssemblyInfo.cs
</commit_message>
<xml_diff>
--- a/Docs/【彭工】关于二段式收费和潮汐收费的原理性解释文档.xlsx
+++ b/Docs/【彭工】关于二段式收费和潮汐收费的原理性解释文档.xlsx
@@ -324,6 +324,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -333,23 +336,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,7 +684,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="10">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -693,7 +693,7 @@
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
@@ -701,23 +701,23 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -726,30 +726,30 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -758,31 +758,31 @@
       <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -794,7 +794,7 @@
       <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E8" t="s">
@@ -802,7 +802,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="10">
         <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -811,19 +811,19 @@
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">

</xml_diff>